<commit_message>
make an action interface update and tweak some code
</commit_message>
<xml_diff>
--- a/MyStoreProject_git/src/test/resources/TestData/AccountCreationTestData.xlsx
+++ b/MyStoreProject_git/src/test/resources/TestData/AccountCreationTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39C0E17-6B75-4AA7-B785-5FF38E754C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061A16FA-9C56-495B-9FDD-35751C43DBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="loginTest" sheetId="2" r:id="rId5"/>
     <sheet name="addToCartPageTest" sheetId="8" r:id="rId6"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId7"/>
-    <sheet name="AccountCreationData" sheetId="7" r:id="rId8"/>
+    <sheet name="accountCreationTest" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -248,19 +248,19 @@
     <t>5</t>
   </si>
   <si>
-    <t>nht@gmail.com</t>
-  </si>
-  <si>
-    <t>qasd21@gmail.com</t>
-  </si>
-  <si>
-    <t>qyr31@gmail.com</t>
-  </si>
-  <si>
     <t>Blouse</t>
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>nht2@gmail.com</t>
+  </si>
+  <si>
+    <t>qhsd21@gmail.com</t>
+  </si>
+  <si>
+    <t>jt1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="16">
         <v>2</v>
@@ -1124,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B12BF8-5AD7-4751-B34C-F337CFF097CA}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="16">
         <v>2</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="15">
         <v>2</v>
@@ -1264,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>66</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>67</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>68</v>

</xml_diff>